<commit_message>
adjusting how months are categorized
</commit_message>
<xml_diff>
--- a/Mobility_data/Other_input/Table_Regressions_to_Run.xlsx
+++ b/Mobility_data/Other_input/Table_Regressions_to_Run.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <t>add_control_bool</t>
   </si>
@@ -207,6 +207,36 @@
   </si>
   <si>
     <t>Regression for daily emissions</t>
+  </si>
+  <si>
+    <t>daily_emissions</t>
+  </si>
+  <si>
+    <t>daily_emissions_noattitude</t>
+  </si>
+  <si>
+    <t>Regression for daily emissions, without attitudinal variables</t>
+  </si>
+  <si>
+    <t>Regression for daily emissions, with additional controls for spatial characteristics</t>
+  </si>
+  <si>
+    <t>daily_emissions_spatial</t>
+  </si>
+  <si>
+    <t>daily_emissions_withbusiness</t>
+  </si>
+  <si>
+    <t>emissions_wege</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regression for daily emissions, including business travels. </t>
+  </si>
+  <si>
+    <t>daily_emissions_control_frequency</t>
+  </si>
+  <si>
+    <t>Regression for daily emissions, when adding a control variables for the use of low-carbon transportation modes</t>
   </si>
 </sst>
 </file>
@@ -531,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,6 +1140,9 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
@@ -1132,6 +1165,125 @@
         <v>0</v>
       </c>
       <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>0</v>
       </c>
     </row>

</xml_diff>